<commit_message>
Updated on May 08
</commit_message>
<xml_diff>
--- a/CoreFramework/testsuitefiles/PortfolioSuite.xlsx
+++ b/CoreFramework/testsuitefiles/PortfolioSuite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -545,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -576,7 +576,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -584,7 +584,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -930,7 +930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>